<commit_message>
melhorado arquivo de especificacao
</commit_message>
<xml_diff>
--- a/Especificação.xlsx
+++ b/Especificação.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Cabeçalho</t>
   </si>
@@ -38,22 +38,85 @@
     <t>Descrição</t>
   </si>
   <si>
-    <t>Extensao do formato, por padrão é sempre "BIR"</t>
-  </si>
-  <si>
-    <t>Tamanho do Disco</t>
-  </si>
-  <si>
-    <t>tamanho do cluster</t>
-  </si>
-  <si>
-    <t>deslocamento até FAT</t>
-  </si>
-  <si>
-    <t>deslocamento até data</t>
-  </si>
-  <si>
-    <t>capacidade de armazenamento</t>
+    <t>Extensao do formato, por padrão é sempre "BI"</t>
+  </si>
+  <si>
+    <t>Tamanho =</t>
+  </si>
+  <si>
+    <t>Tamanho do cluster</t>
+  </si>
+  <si>
+    <t>tamanho do disco</t>
+  </si>
+  <si>
+    <t>inicio da FAT</t>
+  </si>
+  <si>
+    <t>tamanho da FAT</t>
+  </si>
+  <si>
+    <t>inicio dos blocos</t>
+  </si>
+  <si>
+    <t>tamanho dos blocos</t>
+  </si>
+  <si>
+    <t>FAT</t>
+  </si>
+  <si>
+    <t>nome do arquivo</t>
+  </si>
+  <si>
+    <t>primeiro cluster</t>
+  </si>
+  <si>
+    <t>tipo  (pasta ou arquivo)</t>
+  </si>
+  <si>
+    <t>extensao</t>
+  </si>
+  <si>
+    <t>cluster atual</t>
+  </si>
+  <si>
+    <t>cluster pai</t>
+  </si>
+  <si>
+    <t>Alocado ou livre (0 para livre, -1 para final da lista, qualquer outro valor para endereço do cluster</t>
+  </si>
+  <si>
+    <t>4* numero de clusters</t>
+  </si>
+  <si>
+    <t>Dados</t>
+  </si>
+  <si>
+    <t>Lista de Diretórios</t>
+  </si>
+  <si>
+    <t>Arquivo</t>
+  </si>
+  <si>
+    <t>1 cluster</t>
+  </si>
+  <si>
+    <t>EX</t>
+  </si>
+  <si>
+    <t>tamanho em bytes =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tamanho disco = </t>
+  </si>
+  <si>
+    <t>MB</t>
+  </si>
+  <si>
+    <t>k =</t>
+  </si>
+  <si>
+    <t>numero de clusters possiveis</t>
   </si>
 </sst>
 </file>
@@ -69,7 +132,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -88,8 +151,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -112,15 +199,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -133,6 +252,39 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,109 +599,364 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="69.85546875" customWidth="1"/>
+    <col min="3" max="3" width="88.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="D2" s="8"/>
+      <c r="E2" s="9"/>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2">
+        <v>256</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>0</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3">
+        <f>M2 * 1024 * 1024</f>
+        <v>268435456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <f>A3+B3</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="5">
+        <v>4</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
+      <c r="F4">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4">
+        <f>1024*F4</f>
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <f t="shared" ref="A5:A9" si="0">A4+B4</f>
+        <v>6</v>
+      </c>
+      <c r="B5" s="5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+      <c r="H5">
+        <f>L3</f>
+        <v>268435456</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B6" s="5">
+        <v>4</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9"/>
+      <c r="H6">
+        <f>E9</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B7" s="5">
+        <v>4</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9"/>
+      <c r="H7">
+        <f>H13</f>
+        <v>131068</v>
+      </c>
+      <c r="J7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M7">
+        <f>ROUNDDOWN((L3-E9-1)/H4,0)</f>
+        <v>32767</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B8" s="5">
+        <v>4</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="9"/>
+      <c r="H8">
+        <f>H7+E9</f>
+        <v>131094</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B9" s="5">
+        <v>4</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="9">
+        <f>A9+B9</f>
+        <v>26</v>
+      </c>
+      <c r="H9">
+        <f>H5-H8</f>
+        <v>268304362</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H10" s="21"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="I11" s="21"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <f>A3+B3</f>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <f>A9+B9</f>
+        <v>26</v>
+      </c>
+      <c r="B13" s="14">
+        <v>4</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13">
+        <f>M7*4</f>
+        <v>131068</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
+        <f>A13+H13</f>
+        <v>131094</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="20"/>
+      <c r="B18" s="19">
+        <v>16</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="20">
+        <f>A18+B18</f>
+        <v>16</v>
+      </c>
+      <c r="B19" s="19">
         <v>3</v>
       </c>
-      <c r="B4" s="6">
-        <v>4</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="C19" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="20">
+        <f t="shared" ref="A20:A23" si="1">A19+B19</f>
+        <v>19</v>
+      </c>
+      <c r="B20" s="19">
+        <v>4</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="20">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B21" s="19">
+        <v>1</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="20">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B22" s="19">
+        <v>4</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="20">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="B23" s="19">
+        <v>4</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <f t="shared" ref="A5:A8" si="0">A4+B4</f>
-        <v>7</v>
-      </c>
-      <c r="B5" s="6">
-        <v>4</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B6" s="6">
-        <v>4</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B7" s="6">
-        <v>4</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B8" s="6">
-        <v>4</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="E23" s="9">
+        <f>A23+B23</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="18"/>
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="20"/>
+      <c r="B26" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A17:B17"/>
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A11:C11"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Adicionado classe Padroes; feito método formatar para fat e dados; removido cluster; corrigido xls
</commit_message>
<xml_diff>
--- a/Especificação.xlsx
+++ b/Especificação.xlsx
@@ -83,9 +83,6 @@
     <t>cluster pai</t>
   </si>
   <si>
-    <t>Alocado ou livre (0 para livre, -1 para final da lista, qualquer outro valor para endereço do cluster</t>
-  </si>
-  <si>
     <t>4* numero de clusters</t>
   </si>
   <si>
@@ -117,6 +114,9 @@
   </si>
   <si>
     <t>numero de clusters possiveis</t>
+  </si>
+  <si>
+    <t>Alocado ou livre (0 para livre, -1 para final de arquivo, qualquer outro valor para endereço do cluster</t>
   </si>
 </sst>
 </file>
@@ -252,9 +252,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -276,15 +273,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -602,7 +602,7 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,11 +614,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -630,19 +630,19 @@
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8"/>
       <c r="J2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2">
+        <v>20</v>
+      </c>
+      <c r="N2" t="s">
         <v>27</v>
-      </c>
-      <c r="M2">
-        <v>256</v>
-      </c>
-      <c r="N2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -655,17 +655,17 @@
       <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8"/>
       <c r="H3">
         <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L3">
         <f>M2 * 1024 * 1024</f>
-        <v>268435456</v>
+        <v>20971520</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -679,17 +679,17 @@
       <c r="C4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="8"/>
       <c r="F4">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H4">
         <f>1024*F4</f>
-        <v>8192</v>
+        <v>4096</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -703,11 +703,11 @@
       <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="9"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
       <c r="H5">
         <f>L3</f>
-        <v>268435456</v>
+        <v>20971520</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -721,8 +721,8 @@
       <c r="C6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="9"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8"/>
       <c r="H6">
         <f>E9</f>
         <v>26</v>
@@ -739,18 +739,18 @@
       <c r="C7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="9"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
       <c r="H7">
         <f>H13</f>
-        <v>131068</v>
+        <v>20476</v>
       </c>
       <c r="J7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M7">
-        <f>ROUNDDOWN((L3-E9-1)/H4,0)</f>
-        <v>32767</v>
+        <f>ROUNDDOWN((L3-E9)/H4,0)</f>
+        <v>5119</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -764,11 +764,11 @@
       <c r="C8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="8"/>
       <c r="H8">
         <f>H7+E9</f>
-        <v>131094</v>
+        <v>20502</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -782,34 +782,34 @@
       <c r="C9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <f>A9+B9</f>
         <v>26</v>
       </c>
       <c r="H9">
         <f>H5-H8</f>
-        <v>268304362</v>
+        <v>20951018</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H10" s="21"/>
+      <c r="H10" s="18"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="I11" s="21"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="I11" s="18"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -817,52 +817,56 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="15">
+      <c r="A13" s="14">
         <f>A9+B9</f>
         <v>26</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="13">
         <v>4</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H13">
         <f>M7*4</f>
-        <v>131068</v>
+        <v>20476</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="H15">
+        <f>L3-E9-H13</f>
+        <v>20951018</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <f>A13+H13</f>
+        <v>20502</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
-        <f>A13+H13</f>
-        <v>131094</v>
-      </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="18"/>
+      <c r="B17" s="21"/>
       <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="19">
+      <c r="A18" s="17"/>
+      <c r="B18" s="16">
         <v>16</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -870,11 +874,11 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="20">
+      <c r="A19" s="17">
         <f>A18+B18</f>
         <v>16</v>
       </c>
-      <c r="B19" s="19">
+      <c r="B19" s="16">
         <v>3</v>
       </c>
       <c r="C19" s="6" t="s">
@@ -882,11 +886,11 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="20">
+      <c r="A20" s="17">
         <f t="shared" ref="A20:A23" si="1">A19+B19</f>
         <v>19</v>
       </c>
-      <c r="B20" s="19">
+      <c r="B20" s="16">
         <v>4</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -894,11 +898,11 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="20">
+      <c r="A21" s="17">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B21" s="19">
+      <c r="B21" s="16">
         <v>1</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -906,11 +910,11 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="20">
+      <c r="A22" s="17">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="B22" s="19">
+      <c r="B22" s="16">
         <v>4</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -918,35 +922,35 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="20">
+      <c r="A23" s="17">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="B23" s="19">
+      <c r="B23" s="16">
         <v>4</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D23" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="8">
         <f>A23+B23</f>
         <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="21"/>
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="17"/>
+      <c r="B26" s="16" t="s">
         <v>23</v>
-      </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="6"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="20"/>
-      <c r="B26" s="19" t="s">
-        <v>24</v>
       </c>
       <c r="C26" s="6"/>
     </row>

</xml_diff>

<commit_message>
Adicionado controle de data; correções no formatador
</commit_message>
<xml_diff>
--- a/Especificação.xlsx
+++ b/Especificação.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>Cabeçalho</t>
   </si>
@@ -238,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -285,6 +285,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -602,7 +603,7 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,6 +839,18 @@
         <v>20476</v>
       </c>
     </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K14">
+        <v>4088</v>
+      </c>
+      <c r="L14" s="22">
+        <v>2</v>
+      </c>
+      <c r="M14">
+        <f>K14/L14</f>
+        <v>2044</v>
+      </c>
+    </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>20</v>
@@ -848,6 +861,17 @@
         <f>L3-E9-H13</f>
         <v>20951018</v>
       </c>
+      <c r="K15">
+        <f>M14</f>
+        <v>2044</v>
+      </c>
+      <c r="L15" s="22">
+        <v>2</v>
+      </c>
+      <c r="M15">
+        <f t="shared" ref="M15:M19" si="1">K15/L15</f>
+        <v>1022</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
@@ -856,27 +880,60 @@
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <f t="shared" ref="K16:K19" si="2">M15</f>
+        <v>1022</v>
+      </c>
+      <c r="L16">
+        <v>2</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="1"/>
+        <v>511</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="21"/>
       <c r="C17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K17">
+        <f t="shared" si="2"/>
+        <v>511</v>
+      </c>
+      <c r="L17">
+        <v>7</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
       <c r="B18" s="16">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K18">
+        <f t="shared" si="2"/>
+        <v>73</v>
+      </c>
+      <c r="L18">
+        <v>73</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <f>A18+B18</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B19" s="16">
         <v>3</v>
@@ -884,11 +941,15 @@
       <c r="C19" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K19">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
-        <f t="shared" ref="A20:A23" si="1">A19+B19</f>
-        <v>19</v>
+        <f t="shared" ref="A20:A23" si="3">A19+B19</f>
+        <v>23</v>
       </c>
       <c r="B20" s="16">
         <v>4</v>
@@ -897,10 +958,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
-        <f t="shared" si="1"/>
-        <v>23</v>
+        <f t="shared" si="3"/>
+        <v>27</v>
       </c>
       <c r="B21" s="16">
         <v>1</v>
@@ -908,11 +969,18 @@
       <c r="C21" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D21" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="8">
+        <f>A21+B21</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="17">
-        <f t="shared" si="1"/>
-        <v>24</v>
+        <f t="shared" si="3"/>
+        <v>28</v>
       </c>
       <c r="B22" s="16">
         <v>4</v>
@@ -920,11 +988,20 @@
       <c r="C22" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <v>20</v>
+      </c>
+      <c r="L22">
+        <v>3</v>
+      </c>
+      <c r="M22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
-        <f t="shared" si="1"/>
-        <v>28</v>
+        <f t="shared" si="3"/>
+        <v>32</v>
       </c>
       <c r="B23" s="16">
         <v>4</v>
@@ -937,17 +1014,17 @@
       </c>
       <c r="E23" s="8">
         <f>A23+B23</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>22</v>
       </c>
       <c r="B25" s="21"/>
       <c r="C25" s="6"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
       <c r="B26" s="16" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Corrigido montagem da EntradaDiretorio
</commit_message>
<xml_diff>
--- a/Especificação.xlsx
+++ b/Especificação.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Projects\trabalho3\"/>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>Cabeçalho</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Alocado ou livre (0 para livre, -1 para final de arquivo, qualquer outro valor para endereço do cluster</t>
+  </si>
+  <si>
+    <t>Tamanho arquivo</t>
   </si>
 </sst>
 </file>
@@ -276,6 +279,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -285,7 +289,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,11 +618,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -799,11 +802,11 @@
       <c r="H10" s="18"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
       <c r="I11" s="18"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -843,7 +846,7 @@
       <c r="K14">
         <v>4088</v>
       </c>
-      <c r="L14" s="22">
+      <c r="L14" s="19">
         <v>2</v>
       </c>
       <c r="M14">
@@ -852,11 +855,11 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
       <c r="H15">
         <f>L3-E9-H13</f>
         <v>20951018</v>
@@ -865,11 +868,11 @@
         <f>M14</f>
         <v>2044</v>
       </c>
-      <c r="L15" s="22">
+      <c r="L15" s="19">
         <v>2</v>
       </c>
       <c r="M15">
-        <f t="shared" ref="M15:M19" si="1">K15/L15</f>
+        <f t="shared" ref="M15:M18" si="1">K15/L15</f>
         <v>1022</v>
       </c>
     </row>
@@ -893,10 +896,10 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="21"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="6"/>
       <c r="K17">
         <f t="shared" si="2"/>
@@ -913,7 +916,7 @@
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
       <c r="B18" s="16">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>13</v>
@@ -933,7 +936,7 @@
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <f>A18+B18</f>
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B19" s="16">
         <v>3</v>
@@ -948,8 +951,8 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
-        <f t="shared" ref="A20:A23" si="3">A19+B19</f>
-        <v>23</v>
+        <f t="shared" ref="A20:A24" si="3">A19+B19</f>
+        <v>19</v>
       </c>
       <c r="B20" s="16">
         <v>4</v>
@@ -961,84 +964,97 @@
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
         <f t="shared" si="3"/>
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B21" s="16">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="8">
-        <f>A21+B21</f>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="17">
         <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="B22" s="16">
+        <v>1</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="8">
+        <f>A22+B22</f>
         <v>28</v>
-      </c>
-      <c r="B22" s="16">
-        <v>4</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K22">
-        <v>20</v>
-      </c>
-      <c r="L22">
-        <v>3</v>
-      </c>
-      <c r="M22">
-        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
         <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="B23" s="16">
+        <v>4</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K23">
+        <v>20</v>
+      </c>
+      <c r="L23">
+        <v>3</v>
+      </c>
+      <c r="M23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="17">
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
-      <c r="B23" s="16">
-        <v>4</v>
-      </c>
-      <c r="C23" s="6" t="s">
+      <c r="B24" s="16">
+        <v>4</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D24" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="8">
-        <f>A23+B23</f>
+      <c r="E24" s="8">
+        <f>A24+B24</f>
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="6"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="22"/>
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="17"/>
+      <c r="B27" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="6"/>
+      <c r="C27" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A11:C11"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Corrigido gravar nome do arquivo no diretorio
</commit_message>
<xml_diff>
--- a/Especificação.xlsx
+++ b/Especificação.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -606,7 +606,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,6 +844,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K14">
+        <f>H19*E22</f>
         <v>4088</v>
       </c>
       <c r="L14" s="19">
@@ -943,6 +944,14 @@
       </c>
       <c r="C19" s="6" t="s">
         <v>16</v>
+      </c>
+      <c r="H19">
+        <f>ROUNDDOWN(H4/E22,0)</f>
+        <v>146</v>
+      </c>
+      <c r="I19">
+        <f>H19*E22+B23+B24</f>
+        <v>4096</v>
       </c>
       <c r="K19">
         <f t="shared" si="2"/>

</xml_diff>